<commit_message>
Fix BOM and SCH Template
</commit_message>
<xml_diff>
--- a/Project Files/_ClientName_/_ProjectName_/V1I1/Templates/BOM/BOM Purchase PATCH Live.xlsx
+++ b/Project Files/_ClientName_/_ProjectName_/V1I1/Templates/BOM/BOM Purchase PATCH Live.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pa\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PA\Desktop\PATECH-PCB-Template-Project-main\Project Files\_ClientName_\_ProjectName_\V1I1\Templates\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A0FC232-C8F7-471F-BFAD-C30363F62F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7ACE9A-1E2A-4212-8358-80BA138E7911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part List Report" sheetId="3" r:id="rId1"/>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-C09]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
@@ -1212,6 +1212,9 @@
     <xf numFmtId="2" fontId="8" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
@@ -1224,9 +1227,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1726,14 +1726,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1897,13 +1897,13 @@
       <c r="H7" s="25"/>
       <c r="I7" s="87"/>
       <c r="J7" s="25"/>
-      <c r="K7" s="106" t="s">
+      <c r="K7" s="102" t="s">
         <v>58</v>
       </c>
       <c r="L7" s="48"/>
       <c r="M7" s="48"/>
-      <c r="N7" s="77"/>
-      <c r="O7" s="1"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="77"/>
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="68"/>
@@ -1913,11 +1913,11 @@
       </c>
       <c r="D8" s="27">
         <f ca="1">TODAY()</f>
-        <v>44943</v>
+        <v>45158</v>
       </c>
       <c r="E8" s="28">
         <f ca="1">NOW()</f>
-        <v>44943.834578703703</v>
+        <v>45158.799414351852</v>
       </c>
       <c r="F8" s="48"/>
       <c r="G8" s="25"/>
@@ -2063,10 +2063,10 @@
     </row>
     <row r="14" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="68"/>
-      <c r="B14" s="102" t="s">
+      <c r="B14" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="102"/>
+      <c r="C14" s="103"/>
       <c r="D14" s="7"/>
       <c r="E14" s="9"/>
       <c r="F14" s="62" t="s">
@@ -2100,11 +2100,11 @@
         <v>50</v>
       </c>
       <c r="K15" s="48"/>
-      <c r="L15" s="103">
+      <c r="L15" s="104">
         <f>N13</f>
         <v>0</v>
       </c>
-      <c r="M15" s="104"/>
+      <c r="M15" s="105"/>
       <c r="N15" s="56" t="s">
         <v>51</v>
       </c>
@@ -2124,11 +2124,11 @@
         <v>55</v>
       </c>
       <c r="K16" s="8"/>
-      <c r="L16" s="105" t="e">
+      <c r="L16" s="106" t="e">
         <f>L15/H15</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M16" s="105"/>
+      <c r="M16" s="106"/>
       <c r="N16" s="98" t="s">
         <v>51</v>
       </c>
@@ -2184,12 +2184,11 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="K7" r:id="rId1"/>
+    <hyperlink ref="K7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.47244094488188981" right="0.35433070866141736" top="0.59055118110236227" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="57" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="59" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
   <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;LCreated by FEDEVEL&amp;CMotherboard, Processor and Microcontroller Board Design&amp;Rhttp://www.fedevel.com</oddHeader>
     <oddFooter>&amp;C&amp;D&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId3"/>
@@ -2197,7 +2196,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B14"/>
   <sheetViews>

</xml_diff>